<commit_message>
data entry file in sql server
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames/>
+  <calcPr calcId="122211" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,13 +48,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -343,36 +411,212 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="40" customWidth="1" min="6" max="6"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>NAME OF ITEM</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quentiy </t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Form Number</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Contact Number</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Email id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>purna</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>9848165652</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>purnakarki65652@gmail.com</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ktm</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>kbhj</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>kjlkj</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>89431</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>jhvg@gmail.com</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>k;jhnjkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ljknklj</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lm</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>21321</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>321321321</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>knmlnm@gmail.com</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>,/n.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>